<commit_message>
Major refactoring. Renaming references. Create core phylogenies.
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -1,28 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EFDAFA-D89A-1C44-9579-1283D9C5835F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="7440" windowWidth="18940" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="460" windowWidth="11920" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="52">
   <si>
     <t>referenceName</t>
   </si>
@@ -54,88 +61,13 @@
     <t>NS2-P</t>
   </si>
   <si>
-    <t>REF_CPV</t>
-  </si>
-  <si>
-    <t>REF_MVM1</t>
-  </si>
-  <si>
-    <t>REF_PPV</t>
-  </si>
-  <si>
-    <t>REF_MpBuV</t>
-  </si>
-  <si>
-    <t>REF_AMDV</t>
-  </si>
-  <si>
-    <t>REF_ChPV</t>
-  </si>
-  <si>
-    <t>REF_BPV</t>
-  </si>
-  <si>
     <t>REF_PBoV</t>
   </si>
   <si>
     <t>REF_CMV</t>
   </si>
   <si>
-    <t>REF_AAV2</t>
-  </si>
-  <si>
-    <t>REF_SnakePV</t>
-  </si>
-  <si>
-    <t>REF_CAV</t>
-  </si>
-  <si>
-    <t>REF_GPV</t>
-  </si>
-  <si>
-    <t>REF_MDPV</t>
-  </si>
-  <si>
-    <t>REF_B19</t>
-  </si>
-  <si>
     <t>REF_BPV2</t>
-  </si>
-  <si>
-    <t>REF_HamsterPV</t>
-  </si>
-  <si>
-    <t>REF_Mk-PV</t>
-  </si>
-  <si>
-    <t>REF_AAV3</t>
-  </si>
-  <si>
-    <t>REF_AAV4</t>
-  </si>
-  <si>
-    <t>REF_AAV5</t>
-  </si>
-  <si>
-    <t>REF_AAV6</t>
-  </si>
-  <si>
-    <t>REF_AAV7</t>
-  </si>
-  <si>
-    <t>REF_AAV8</t>
-  </si>
-  <si>
-    <t>REF_AAV9</t>
-  </si>
-  <si>
-    <t>REF_AAV10</t>
-  </si>
-  <si>
-    <t>REF_AAV11</t>
-  </si>
-  <si>
-    <t>REF_AAV12</t>
   </si>
   <si>
     <t>NS1</t>
@@ -147,22 +79,10 @@
     <t>CP</t>
   </si>
   <si>
-    <t>REF_FCDNV</t>
-  </si>
-  <si>
-    <t>REF_AAV1</t>
-  </si>
-  <si>
-    <t>REF_Zsana</t>
-  </si>
-  <si>
     <t>ORF7</t>
   </si>
   <si>
     <t>ORF5</t>
-  </si>
-  <si>
-    <t>REF_BdrPV</t>
   </si>
   <si>
     <t>AAP</t>
@@ -170,12 +90,108 @@
   <si>
     <t>REF_PfDNV</t>
   </si>
+  <si>
+    <t>whole_genome</t>
+  </si>
+  <si>
+    <t>REF_Proto_MASTER_CPV</t>
+  </si>
+  <si>
+    <t>REF_Amdo_MASTER_AMDV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_MASTER_AAV2</t>
+  </si>
+  <si>
+    <t>REF_Erythro_MASTER_B19</t>
+  </si>
+  <si>
+    <t>REF_Ave_MASTER_ChPV</t>
+  </si>
+  <si>
+    <t>REF_Tetra_MASTER_EhBtPV1</t>
+  </si>
+  <si>
+    <t>REF_Proto_PPV</t>
+  </si>
+  <si>
+    <t>REF_Proto_MpBuV</t>
+  </si>
+  <si>
+    <t>REF_Boca_MASTER_BPV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV3</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV4</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV5</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV6</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV7</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV8</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV9</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV10</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV11</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV12</t>
+  </si>
+  <si>
+    <t>REF_Dependo_AAV1</t>
+  </si>
+  <si>
+    <t>REF_Dependo_SnakePV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_CAV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_GPV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_MDPV</t>
+  </si>
+  <si>
+    <t>REF_Erythro_Chipmunk-PV</t>
+  </si>
+  <si>
+    <t>REF_Dependo_BdrPV</t>
+  </si>
+  <si>
+    <t>REF_Proto_Zsana</t>
+  </si>
+  <si>
+    <t>REF_Chappa_Mk-PV</t>
+  </si>
+  <si>
+    <t>REF_Hepandenso_MASTER_FCDNV</t>
+  </si>
+  <si>
+    <t>REF_Proto_HamsterPV</t>
+  </si>
+  <si>
+    <t>REF_Proto_MVM1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +231,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -237,7 +259,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -1986,14 +2008,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2009,6 +2030,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1733">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -3751,6 +3775,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4076,1752 +4103,1877 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1520"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A87" sqref="A85:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12" style="10" customWidth="1"/>
+    <col min="4" max="4" width="12" style="9" customWidth="1"/>
     <col min="5" max="5" width="31.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="4">
         <v>130</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D4" s="7">
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>466</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D5" s="7">
         <v>969</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4">
-        <v>114</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2279</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4">
-        <v>2399</v>
-      </c>
-      <c r="D6" s="8">
-        <v>4555</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4">
-        <v>292</v>
-      </c>
-      <c r="D7" s="8">
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>114</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4">
+        <v>2399</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>5075</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>292</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
         <v>2388</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D11" s="8">
         <v>4547</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C12" s="4">
         <v>63</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D12" s="7">
         <v>1982</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C13" s="4">
         <v>2247</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D13" s="7">
         <v>4403</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4">
-        <v>206</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2406</v>
-      </c>
-      <c r="D12" s="8">
-        <v>4349</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4">
-        <v>411</v>
-      </c>
-      <c r="D13" s="8">
-        <v>2495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4">
-        <v>2998</v>
-      </c>
-      <c r="D14" s="8">
-        <v>5025</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="4">
-        <v>740</v>
-      </c>
-      <c r="D15" s="8">
-        <v>2920</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>206</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4">
-        <v>2661</v>
-      </c>
-      <c r="D16" s="8">
-        <v>3302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>2406</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4">
-        <v>3286</v>
-      </c>
-      <c r="D17" s="8">
-        <v>5307</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>5257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="4">
-        <v>149</v>
-      </c>
-      <c r="D18" s="8">
-        <v>2260</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>411</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4">
-        <v>2333</v>
-      </c>
-      <c r="D19" s="8">
-        <v>3019</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>2998</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
-        <v>3003</v>
-      </c>
-      <c r="D20" s="8">
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>5517</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="4">
-        <v>429</v>
-      </c>
-      <c r="D21" s="8">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>740</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="4">
-        <v>2389</v>
-      </c>
-      <c r="D22" s="8">
-        <v>2949</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>2661</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="4">
-        <v>2933</v>
-      </c>
-      <c r="D23" s="8">
-        <v>5044</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>3286</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C25" s="4">
         <v>321</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="7">
         <v>2252</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C26" s="4">
         <v>2203</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="7">
         <v>4410</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C27" s="4">
         <v>318</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D27" s="7">
         <v>2192</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C28" s="4">
         <v>2209</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="7">
         <v>4419</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="6" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C30" s="4">
         <v>372</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D30" s="7">
         <v>2243</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="6" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C31" s="4">
         <v>2260</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D31" s="7">
         <v>4464</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="6" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C32" s="4">
         <v>359</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D32" s="7">
         <v>2191</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C33" s="4">
         <v>2207</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D33" s="7">
         <v>4381</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C34" s="4">
         <v>320</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D34" s="7">
         <v>2191</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="6" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C35" s="4">
         <v>2208</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D35" s="7">
         <v>4418</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="6" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C36" s="4">
         <v>334</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D36" s="7">
         <v>2205</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="6" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C37" s="4">
         <v>2222</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D37" s="7">
         <v>4435</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="6" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C38" s="4">
         <v>227</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D38" s="7">
         <v>2104</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="6" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C39" s="4">
         <v>2121</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D39" s="7">
         <v>4337</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="6" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C40" s="4">
         <v>228</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D40" s="7">
         <v>2099</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="6" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C41" s="4">
         <v>2116</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D41" s="7">
         <v>4329</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="4">
-        <v>1</v>
-      </c>
-      <c r="D40" s="8">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1886</v>
-      </c>
-      <c r="D41" s="8">
-        <v>4102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <v>1869</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="4">
         <v>1886</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="7">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1886</v>
+      </c>
+      <c r="D45" s="7">
         <v>4087</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C46" s="4">
         <v>103</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D46" s="7">
         <v>1968</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="6" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C47" s="4">
         <v>1985</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D47" s="7">
         <v>4213</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="4">
-        <v>324</v>
-      </c>
-      <c r="D46" s="8">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="4">
-        <v>2030</v>
-      </c>
-      <c r="D47" s="8">
-        <v>4210</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="4">
-        <v>347</v>
-      </c>
-      <c r="D48" s="8">
-        <v>2179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>324</v>
+      </c>
+      <c r="D48" s="7">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="4">
-        <v>2195</v>
-      </c>
-      <c r="D49" s="8">
-        <v>4375</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>2030</v>
+      </c>
+      <c r="D49" s="7">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="4">
-        <v>537</v>
-      </c>
-      <c r="D50" s="8">
-        <v>2420</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>347</v>
+      </c>
+      <c r="D50" s="7">
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="4">
-        <v>2439</v>
-      </c>
-      <c r="D51" s="8">
-        <v>4637</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>2195</v>
+      </c>
+      <c r="D51" s="7">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C52" s="4">
-        <v>548</v>
-      </c>
-      <c r="D52" s="8">
-        <v>2431</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>537</v>
+      </c>
+      <c r="D52" s="7">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="4">
-        <v>2450</v>
-      </c>
-      <c r="D53" s="8">
-        <v>4648</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>2439</v>
+      </c>
+      <c r="D53" s="7">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="4">
-        <v>616</v>
-      </c>
-      <c r="D54" s="8">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>548</v>
+      </c>
+      <c r="D54" s="7">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="4">
+        <v>2450</v>
+      </c>
+      <c r="D55" s="7">
+        <v>4648</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="7">
+        <v>5596</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="4">
+        <v>616</v>
+      </c>
+      <c r="D57" s="7">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="4">
         <v>2624</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D58" s="7">
         <v>4969</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="7">
+        <v>5097</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="4">
-        <v>306</v>
-      </c>
-      <c r="D56" s="8">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" s="4" t="s">
+      <c r="C60" s="4">
+        <v>198</v>
+      </c>
+      <c r="D60" s="7">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="4">
-        <v>2268</v>
-      </c>
-      <c r="D57" s="8">
-        <v>5384</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="4" t="s">
+      <c r="C61" s="4">
+        <v>2511</v>
+      </c>
+      <c r="D61" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+      <c r="D62" s="7">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C63" s="4">
         <v>122</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D63" s="7">
         <v>2140</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C64" s="4">
         <v>2664</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D64" s="7">
         <v>4427</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="4">
+        <v>1</v>
+      </c>
+      <c r="D65" s="7">
+        <v>4442</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C66" s="4">
         <v>2110</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D66" s="7">
         <v>2727</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="4">
-        <v>811</v>
-      </c>
-      <c r="D61" s="8">
-        <v>2790</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="4">
-        <v>2006</v>
-      </c>
-      <c r="D62" s="8">
-        <v>2725</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="4">
-        <v>2783</v>
-      </c>
-      <c r="D63" s="8">
-        <v>4273</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" s="4">
-        <v>62</v>
-      </c>
-      <c r="D64" s="10">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" s="4">
-        <v>1330</v>
-      </c>
-      <c r="D65" s="10">
-        <v>3066</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66" s="4">
-        <v>3493</v>
-      </c>
-      <c r="D66" s="10">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="4" t="s">
-        <v>42</v>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="4">
-        <v>335</v>
-      </c>
-      <c r="D67" s="4">
-        <v>2206</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="4" t="s">
-        <v>42</v>
+        <v>811</v>
+      </c>
+      <c r="D67" s="7">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D68" s="7">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="4">
-        <v>2223</v>
-      </c>
-      <c r="D68" s="4">
-        <v>4433</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>43</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C69" s="4">
+        <v>2783</v>
+      </c>
+      <c r="D69" s="7">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="4">
         <v>1</v>
       </c>
-      <c r="D69" s="10">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="4">
-        <v>1883</v>
-      </c>
-      <c r="D70" s="10">
-        <v>2272</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>43</v>
+      <c r="D70" s="7">
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C71" s="4">
-        <v>2668</v>
-      </c>
-      <c r="D71" s="10">
-        <v>4281</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>48</v>
+        <v>62</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C72" s="4">
-        <v>202</v>
-      </c>
-      <c r="D72" s="10">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="14" customHeight="1">
-      <c r="A73" t="s">
-        <v>48</v>
+        <v>1330</v>
+      </c>
+      <c r="D72" s="7">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C73" s="4">
-        <v>965</v>
-      </c>
-      <c r="D73" s="10">
-        <v>2689</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>48</v>
+        <v>3493</v>
+      </c>
+      <c r="D73" s="7">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C74" s="4">
-        <v>969</v>
-      </c>
-      <c r="D74" s="10">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="D74" s="11">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C75" s="4">
-        <v>2719</v>
-      </c>
-      <c r="D75" s="10">
-        <v>4335</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
+        <v>335</v>
+      </c>
+      <c r="D75" s="4">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="4">
+        <v>2223</v>
+      </c>
+      <c r="D76" s="4">
+        <v>4433</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="4">
+        <v>1</v>
+      </c>
+      <c r="D77" s="4">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78" s="7">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="4">
+        <v>1883</v>
+      </c>
+      <c r="D79" s="7">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="4">
+        <v>2668</v>
+      </c>
+      <c r="D80" s="7">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C76">
+      <c r="B81" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="4">
+        <v>1</v>
+      </c>
+      <c r="D81" s="11">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" s="4">
         <v>2594</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D82" s="7">
         <v>3127</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C77">
+      <c r="C83" s="4">
         <v>386</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D83" s="7">
         <v>2083</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C78">
+      <c r="C84" s="4">
         <v>2101</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D84" s="7">
         <v>4278</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="16" customHeight="1"/>
-    <row r="88" spans="1:2">
-      <c r="A88" s="2"/>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="2"/>
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1</v>
+      </c>
+      <c r="D85" s="7">
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="4">
+        <v>174</v>
+      </c>
+      <c r="D86" s="7">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="4">
+        <v>2279</v>
+      </c>
+      <c r="D87" s="7">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="1"/>
-      <c r="D97" s="11"/>
-    </row>
-    <row r="98" spans="1:4">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="1"/>
-      <c r="D98" s="11"/>
-    </row>
-    <row r="99" spans="1:4">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="D100" s="10"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="D101" s="10"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-    </row>
-    <row r="120" spans="1:3">
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="1"/>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="1"/>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
-      <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="1:3">
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="1"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="1"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="1"/>
-      <c r="E133" s="2"/>
-    </row>
-    <row r="134" spans="1:5">
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="1"/>
-      <c r="E134" s="2"/>
-    </row>
-    <row r="135" spans="1:5">
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="1"/>
-      <c r="E135" s="2"/>
-    </row>
-    <row r="136" spans="1:5">
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="1"/>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="1"/>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="1"/>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="1"/>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="1"/>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="1"/>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
       <c r="B151" s="1"/>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="1"/>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="1"/>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
       <c r="B154" s="1"/>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
       <c r="B155" s="1"/>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="2"/>
       <c r="B156" s="1"/>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="2"/>
       <c r="B157" s="1"/>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="1"/>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="1"/>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="1"/>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="1"/>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
       <c r="B162" s="1"/>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="1"/>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="1"/>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="1"/>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
       <c r="B166" s="1"/>
     </row>
-    <row r="184" spans="5:5">
-      <c r="E184" s="1"/>
-    </row>
-    <row r="185" spans="5:5">
-      <c r="E185" s="1"/>
-    </row>
-    <row r="186" spans="5:5">
-      <c r="E186" s="1"/>
-    </row>
-    <row r="187" spans="5:5">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="2"/>
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="2"/>
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="2"/>
+      <c r="B169" s="1"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E187" s="1"/>
     </row>
-    <row r="188" spans="5:5">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E188" s="1"/>
     </row>
-    <row r="189" spans="5:5">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E189" s="1"/>
     </row>
-    <row r="242" spans="1:2">
-      <c r="A242" s="2"/>
-      <c r="B242" s="1"/>
-    </row>
-    <row r="243" spans="1:2">
-      <c r="A243" s="2"/>
-      <c r="B243" s="1"/>
-    </row>
-    <row r="244" spans="1:2">
-      <c r="A244" s="2"/>
-      <c r="B244" s="1"/>
-    </row>
-    <row r="245" spans="1:2">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E190" s="1"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E191" s="1"/>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E192" s="1"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="2"/>
       <c r="B245" s="1"/>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="2"/>
       <c r="B246" s="1"/>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="2"/>
       <c r="B247" s="1"/>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="2"/>
       <c r="B248" s="1"/>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="2"/>
       <c r="B249" s="1"/>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="2"/>
       <c r="B250" s="1"/>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
       <c r="B251" s="1"/>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="2"/>
       <c r="B252" s="1"/>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="2"/>
       <c r="B253" s="1"/>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="2"/>
       <c r="B254" s="1"/>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="2"/>
       <c r="B255" s="1"/>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="2"/>
       <c r="B256" s="1"/>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="2"/>
       <c r="B257" s="1"/>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="2"/>
       <c r="B258" s="1"/>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
       <c r="B259" s="1"/>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="2"/>
       <c r="B260" s="1"/>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="2"/>
       <c r="B261" s="1"/>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="2"/>
       <c r="B262" s="1"/>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="2"/>
       <c r="B263" s="1"/>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="2"/>
       <c r="B264" s="1"/>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="2"/>
       <c r="B265" s="1"/>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="2"/>
-    </row>
-    <row r="267" spans="1:2">
+      <c r="B266" s="1"/>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="2"/>
       <c r="B267" s="1"/>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="2"/>
       <c r="B268" s="1"/>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="2"/>
-      <c r="B269" s="1"/>
-    </row>
-    <row r="270" spans="1:2">
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="2"/>
       <c r="B270" s="1"/>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="2"/>
       <c r="B271" s="1"/>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="2"/>
       <c r="B272" s="1"/>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="2"/>
       <c r="B273" s="1"/>
     </row>
-    <row r="956" spans="3:3">
-      <c r="C956" s="2"/>
-    </row>
-    <row r="1092" spans="1:1">
-      <c r="A1092" s="2"/>
-    </row>
-    <row r="1093" spans="1:1">
-      <c r="A1093" s="2"/>
-    </row>
-    <row r="1218" spans="1:1">
-      <c r="A1218" s="2"/>
-    </row>
-    <row r="1219" spans="1:1">
-      <c r="A1219" s="2"/>
-    </row>
-    <row r="1220" spans="1:1">
-      <c r="A1220" s="2"/>
-    </row>
-    <row r="1221" spans="1:1">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="2"/>
+      <c r="B274" s="1"/>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="2"/>
+      <c r="B275" s="1"/>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="2"/>
+      <c r="B276" s="1"/>
+    </row>
+    <row r="959" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C959" s="2"/>
+    </row>
+    <row r="1095" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1095" s="2"/>
+    </row>
+    <row r="1096" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1096" s="2"/>
+    </row>
+    <row r="1221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1221" s="2"/>
     </row>
-    <row r="1222" spans="1:1">
+    <row r="1222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1222" s="2"/>
     </row>
-    <row r="1223" spans="1:1">
+    <row r="1223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1223" s="2"/>
     </row>
-    <row r="1268" spans="1:4">
-      <c r="C1268" s="2"/>
-      <c r="D1268" s="11"/>
-    </row>
-    <row r="1269" spans="1:4">
-      <c r="C1269" s="2"/>
-      <c r="D1269" s="11"/>
-    </row>
-    <row r="1270" spans="1:4">
-      <c r="C1270" s="2"/>
-      <c r="D1270" s="11"/>
-    </row>
-    <row r="1272" spans="1:4">
-      <c r="A1272" s="2"/>
-    </row>
-    <row r="1273" spans="1:4">
-      <c r="A1273" s="2"/>
-    </row>
-    <row r="1274" spans="1:4">
-      <c r="A1274" s="2"/>
-    </row>
-    <row r="1275" spans="1:4">
+    <row r="1224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1224" s="2"/>
+    </row>
+    <row r="1225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1225" s="2"/>
+    </row>
+    <row r="1226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1226" s="2"/>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1271" s="2"/>
+      <c r="D1271" s="10"/>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1272" s="2"/>
+      <c r="D1272" s="10"/>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1273" s="2"/>
+      <c r="D1273" s="10"/>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1275" s="2"/>
     </row>
-    <row r="1276" spans="1:4">
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1276" s="2"/>
     </row>
-    <row r="1295" spans="1:1">
-      <c r="A1295" s="2"/>
-    </row>
-    <row r="1296" spans="1:1">
-      <c r="A1296" s="2"/>
-    </row>
-    <row r="1297" spans="1:1">
-      <c r="A1297" s="2"/>
-    </row>
-    <row r="1298" spans="1:1">
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1277" s="2"/>
+    </row>
+    <row r="1278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1278" s="2"/>
+    </row>
+    <row r="1279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1279" s="2"/>
+    </row>
+    <row r="1298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1298" s="2"/>
     </row>
-    <row r="1299" spans="1:1">
+    <row r="1299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1299" s="2"/>
     </row>
-    <row r="1300" spans="1:1">
+    <row r="1300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1300" s="2"/>
     </row>
-    <row r="1301" spans="1:1">
+    <row r="1301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1301" s="2"/>
     </row>
-    <row r="1303" spans="1:1">
+    <row r="1302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1302" s="2"/>
+    </row>
+    <row r="1303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1303" s="2"/>
     </row>
-    <row r="1304" spans="1:1">
+    <row r="1304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1304" s="2"/>
     </row>
-    <row r="1305" spans="1:1">
-      <c r="A1305" s="2"/>
-    </row>
-    <row r="1306" spans="1:1">
+    <row r="1306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1306" s="2"/>
     </row>
-    <row r="1307" spans="1:1">
+    <row r="1307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1307" s="2"/>
     </row>
-    <row r="1308" spans="1:1">
+    <row r="1308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1308" s="2"/>
     </row>
-    <row r="1360" spans="1:1">
-      <c r="A1360" s="2"/>
-    </row>
-    <row r="1361" spans="1:1">
-      <c r="A1361" s="2"/>
-    </row>
-    <row r="1362" spans="1:1">
-      <c r="A1362" s="2"/>
-    </row>
-    <row r="1363" spans="1:1">
+    <row r="1309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1309" s="2"/>
+    </row>
+    <row r="1310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1310" s="2"/>
+    </row>
+    <row r="1311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1311" s="2"/>
+    </row>
+    <row r="1363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1363" s="2"/>
     </row>
-    <row r="1365" spans="1:1">
+    <row r="1364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1364" s="2"/>
+    </row>
+    <row r="1365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1365" s="2"/>
     </row>
-    <row r="1366" spans="1:1">
+    <row r="1366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1366" s="2"/>
     </row>
-    <row r="1367" spans="1:1">
-      <c r="A1367" s="2"/>
-    </row>
-    <row r="1368" spans="1:1">
+    <row r="1368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1368" s="2"/>
     </row>
-    <row r="1403" spans="1:1">
-      <c r="A1403" s="2"/>
-    </row>
-    <row r="1404" spans="1:1">
-      <c r="A1404" s="2"/>
-    </row>
-    <row r="1405" spans="1:1">
-      <c r="A1405" s="2"/>
-    </row>
-    <row r="1406" spans="1:1">
+    <row r="1369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1369" s="2"/>
+    </row>
+    <row r="1370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1370" s="2"/>
+    </row>
+    <row r="1371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1371" s="2"/>
+    </row>
+    <row r="1406" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1406" s="2"/>
     </row>
-    <row r="1407" spans="1:1">
+    <row r="1407" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1407" s="2"/>
     </row>
-    <row r="1408" spans="1:1">
+    <row r="1408" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1408" s="2"/>
     </row>
-    <row r="1450" spans="2:4">
-      <c r="C1450" s="2"/>
-      <c r="D1450" s="11"/>
-    </row>
-    <row r="1451" spans="2:4">
-      <c r="B1451" s="2"/>
-      <c r="C1451" s="2"/>
-      <c r="D1451" s="11"/>
-    </row>
-    <row r="1452" spans="2:4">
-      <c r="B1452" s="2"/>
-      <c r="C1452" s="2"/>
-      <c r="D1452" s="11"/>
-    </row>
-    <row r="1453" spans="2:4">
-      <c r="B1453" s="2"/>
+    <row r="1409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1409" s="2"/>
+    </row>
+    <row r="1410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1410" s="2"/>
+    </row>
+    <row r="1411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1411" s="2"/>
+    </row>
+    <row r="1453" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C1453" s="2"/>
-      <c r="D1453" s="11"/>
-    </row>
-    <row r="1454" spans="2:4">
+      <c r="D1453" s="10"/>
+    </row>
+    <row r="1454" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1454" s="2"/>
       <c r="C1454" s="2"/>
-      <c r="D1454" s="11"/>
-    </row>
-    <row r="1517" spans="1:1">
-      <c r="A1517" s="2"/>
-    </row>
-    <row r="1518" spans="1:1">
-      <c r="A1518" s="2"/>
-    </row>
-    <row r="1519" spans="1:1">
-      <c r="A1519" s="2"/>
-    </row>
-    <row r="1520" spans="1:1">
+      <c r="D1454" s="10"/>
+    </row>
+    <row r="1455" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1455" s="2"/>
+      <c r="C1455" s="2"/>
+      <c r="D1455" s="10"/>
+    </row>
+    <row r="1456" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1456" s="2"/>
+      <c r="C1456" s="2"/>
+      <c r="D1456" s="10"/>
+    </row>
+    <row r="1457" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C1457" s="2"/>
+      <c r="D1457" s="10"/>
+    </row>
+    <row r="1520" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1520" s="2"/>
+    </row>
+    <row r="1521" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1521" s="2"/>
+    </row>
+    <row r="1522" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1522" s="2"/>
+    </row>
+    <row r="1523" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1523" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5832,4 +5984,201 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4035936-3065-7A4B-90CB-A32C5DA75E1A}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2333</v>
+      </c>
+      <c r="D1" s="7">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3003</v>
+      </c>
+      <c r="D2" s="7">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>429</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2389</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2933</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
+        <v>202</v>
+      </c>
+      <c r="D6" s="7">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>5454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>965</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>969</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2719</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>306</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2268</v>
+      </c>
+      <c r="D13" s="7">
+        <v>5384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring for phylogeny build
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EFDAFA-D89A-1C44-9579-1283D9C5835F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2ECB0C-2AC5-2140-8319-E0A9926926B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="460" windowWidth="11920" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="54">
   <si>
     <t>referenceName</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>REF_Proto_MVM1</t>
+  </si>
+  <si>
+    <t>Rep78</t>
+  </si>
+  <si>
+    <t>VP1</t>
   </si>
 </sst>
 </file>
@@ -4106,8 +4112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A87" sqref="A85:XFD87"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4168,7 +4174,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4">
         <v>130</v>
@@ -4182,7 +4188,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4">
         <v>466</v>
@@ -4210,7 +4216,7 @@
         <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C7" s="4">
         <v>114</v>
@@ -4224,7 +4230,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4">
         <v>2399</v>
@@ -4252,7 +4258,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4">
         <v>292</v>
@@ -4266,7 +4272,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C11" s="4">
         <v>2388</v>
@@ -4280,7 +4286,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C12" s="4">
         <v>63</v>
@@ -4294,7 +4300,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4">
         <v>2247</v>
@@ -4322,7 +4328,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C15" s="4">
         <v>206</v>
@@ -4336,7 +4342,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4">
         <v>2406</v>
@@ -4364,7 +4370,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4">
         <v>411</v>
@@ -4378,7 +4384,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4">
         <v>2998</v>
@@ -4406,7 +4412,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4">
         <v>740</v>
@@ -4434,7 +4440,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4">
         <v>3286</v>
@@ -4462,7 +4468,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C25" s="4">
         <v>321</v>
@@ -4476,7 +4482,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C26" s="4">
         <v>2203</v>
@@ -4490,7 +4496,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4">
         <v>318</v>
@@ -4504,7 +4510,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C28" s="4">
         <v>2209</v>
@@ -4531,8 +4537,8 @@
       <c r="A30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>4</v>
+      <c r="B30" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C30" s="4">
         <v>372</v>
@@ -4546,7 +4552,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C31" s="4">
         <v>2260</v>
@@ -4559,8 +4565,8 @@
       <c r="A32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>4</v>
+      <c r="B32" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="4">
         <v>359</v>
@@ -4574,7 +4580,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C33" s="4">
         <v>2207</v>
@@ -4587,8 +4593,8 @@
       <c r="A34" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>4</v>
+      <c r="B34" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C34" s="4">
         <v>320</v>
@@ -4602,7 +4608,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C35" s="4">
         <v>2208</v>
@@ -4615,8 +4621,8 @@
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>4</v>
+      <c r="B36" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="4">
         <v>334</v>
@@ -4630,7 +4636,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C37" s="4">
         <v>2222</v>
@@ -4643,8 +4649,8 @@
       <c r="A38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>4</v>
+      <c r="B38" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C38" s="4">
         <v>227</v>
@@ -4658,7 +4664,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C39" s="4">
         <v>2121</v>
@@ -4671,8 +4677,8 @@
       <c r="A40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>4</v>
+      <c r="B40" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C40" s="4">
         <v>228</v>
@@ -4686,7 +4692,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C41" s="4">
         <v>2116</v>
@@ -4699,8 +4705,8 @@
       <c r="A42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>4</v>
+      <c r="B42" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
@@ -4714,7 +4720,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C43" s="4">
         <v>1886</v>
@@ -4727,8 +4733,8 @@
       <c r="A44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>4</v>
+      <c r="B44" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
@@ -4742,7 +4748,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C45" s="4">
         <v>1886</v>
@@ -4755,8 +4761,8 @@
       <c r="A46" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>4</v>
+      <c r="B46" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C46" s="4">
         <v>103</v>
@@ -4770,7 +4776,7 @@
         <v>39</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C47" s="4">
         <v>1985</v>
@@ -4784,7 +4790,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C48" s="4">
         <v>324</v>
@@ -4798,7 +4804,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C49" s="4">
         <v>2030</v>
@@ -4812,7 +4818,7 @@
         <v>42</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C50" s="4">
         <v>347</v>
@@ -4826,7 +4832,7 @@
         <v>42</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C51" s="4">
         <v>2195</v>
@@ -4840,7 +4846,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C52" s="4">
         <v>537</v>
@@ -4854,7 +4860,7 @@
         <v>43</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C53" s="4">
         <v>2439</v>
@@ -4868,7 +4874,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C54" s="4">
         <v>548</v>
@@ -4882,7 +4888,7 @@
         <v>44</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C55" s="4">
         <v>2450</v>
@@ -4924,7 +4930,7 @@
         <v>24</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C58" s="4">
         <v>2624</v>
@@ -4952,7 +4958,7 @@
         <v>45</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C60" s="4">
         <v>198</v>
@@ -4966,7 +4972,7 @@
         <v>45</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C61" s="4">
         <v>2511</v>
@@ -4994,7 +5000,7 @@
         <v>50</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C63" s="4">
         <v>122</v>
@@ -5008,7 +5014,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C64" s="4">
         <v>2664</v>
@@ -5050,7 +5056,7 @@
         <v>48</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C67" s="4">
         <v>811</v>
@@ -5078,7 +5084,7 @@
         <v>48</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C69" s="4">
         <v>2783</v>
@@ -5162,7 +5168,7 @@
         <v>40</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C75" s="4">
         <v>335</v>
@@ -5176,7 +5182,7 @@
         <v>40</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C76" s="4">
         <v>2223</v>
@@ -5204,7 +5210,7 @@
         <v>47</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C78" s="4">
         <v>1</v>
@@ -5232,7 +5238,7 @@
         <v>47</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C80" s="4">
         <v>2668</v>
@@ -5274,7 +5280,7 @@
         <v>46</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C83" s="4">
         <v>386</v>
@@ -5288,7 +5294,7 @@
         <v>46</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C84" s="4">
         <v>2101</v>
@@ -5316,7 +5322,7 @@
         <v>26</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C86" s="4">
         <v>174</v>
@@ -5330,7 +5336,7 @@
         <v>26</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C87" s="4">
         <v>2279</v>

</xml_diff>

<commit_message>
Refactoring of master references / core project
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81181AC8-6D98-5B43-A615-D7AA62269CD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED40722-A69D-F444-8E4E-DCF844758229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19480" yWindow="460" windowWidth="31300" windowHeight="25060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -4109,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4139,8 +4140,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
+      <c r="A2" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -4149,1190 +4150,812 @@
         <v>1</v>
       </c>
       <c r="D2" s="7">
-        <v>5323</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
+      <c r="A3" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>2110</v>
       </c>
       <c r="D3" s="7">
-        <v>130</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
+      <c r="A4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="4">
-        <v>272</v>
+        <v>811</v>
       </c>
       <c r="D4" s="7">
-        <v>2278</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
+      <c r="A5" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="4">
-        <v>2285</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4">
+        <v>2783</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
-        <v>5149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="4">
-        <v>114</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2279</v>
+      <c r="D7" s="11">
+        <v>4718</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
-        <v>2399</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4555</v>
+        <v>335</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2206</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>5075</v>
+        <v>2223</v>
+      </c>
+      <c r="D9" s="4">
+        <v>4433</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="4">
-        <v>292</v>
+        <v>1</v>
       </c>
       <c r="D10" s="7">
-        <v>2280</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="4">
-        <v>2388</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4547</v>
+        <v>1886</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="4">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="D12" s="7">
-        <v>1982</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="4">
-        <v>2247</v>
+        <v>1886</v>
       </c>
       <c r="D13" s="7">
-        <v>4403</v>
+        <v>4087</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D14" s="7">
-        <v>4801</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C15" s="4">
-        <v>206</v>
+        <v>1985</v>
       </c>
       <c r="D15" s="7">
-        <v>1978</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="4">
-        <v>2406</v>
+        <v>318</v>
       </c>
       <c r="D16" s="7">
-        <v>4349</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2209</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="7">
-        <v>5257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="D18" s="7">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="4">
-        <v>411</v>
-      </c>
-      <c r="D18" s="7">
-        <v>2495</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4">
+        <v>372</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4">
-        <v>2998</v>
-      </c>
-      <c r="D19" s="7">
-        <v>5025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>2260</v>
       </c>
       <c r="D20" s="7">
-        <v>5517</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>29</v>
+      <c r="A21" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="4">
-        <v>740</v>
+        <v>359</v>
       </c>
       <c r="D21" s="7">
-        <v>2920</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>7</v>
+      <c r="A22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C22" s="4">
-        <v>2661</v>
+        <v>2207</v>
       </c>
       <c r="D22" s="7">
-        <v>3302</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>29</v>
+      <c r="A23" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4">
+        <v>320</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="4">
-        <v>3286</v>
-      </c>
-      <c r="D23" s="7">
-        <v>5307</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C24" s="4">
-        <v>1</v>
+        <v>2208</v>
       </c>
       <c r="D24" s="7">
-        <v>4679</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="4">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="D25" s="7">
-        <v>2252</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="4">
-        <v>2203</v>
+        <v>2222</v>
       </c>
       <c r="D26" s="7">
-        <v>4410</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="4">
-        <v>318</v>
+        <v>227</v>
       </c>
       <c r="D27" s="7">
-        <v>2192</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="4">
-        <v>2209</v>
+        <v>2121</v>
       </c>
       <c r="D28" s="7">
-        <v>4419</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>31</v>
+      <c r="A29" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="4">
+        <v>228</v>
+      </c>
+      <c r="D29" s="7">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2116</v>
+      </c>
+      <c r="D30" s="7">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D29" s="7">
-        <v>4767</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="D31" s="11">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2594</v>
+      </c>
+      <c r="D32" s="7">
+        <v>3127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="4">
-        <v>372</v>
-      </c>
-      <c r="D30" s="7">
-        <v>2243</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="12" t="s">
+      <c r="C33" s="4">
+        <v>386</v>
+      </c>
+      <c r="D33" s="7">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="4">
-        <v>2260</v>
-      </c>
-      <c r="D31" s="7">
-        <v>4464</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="C34" s="4">
+        <v>2101</v>
+      </c>
+      <c r="D34" s="7">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="4">
-        <v>359</v>
-      </c>
-      <c r="D32" s="7">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2207</v>
-      </c>
-      <c r="D33" s="7">
-        <v>4381</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="4">
-        <v>320</v>
-      </c>
-      <c r="D34" s="7">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="C35" s="4">
-        <v>2208</v>
+        <v>347</v>
       </c>
       <c r="D35" s="7">
-        <v>4418</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C36" s="4">
-        <v>334</v>
+        <v>2195</v>
       </c>
       <c r="D36" s="7">
-        <v>2205</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C37" s="4">
-        <v>2222</v>
+        <v>537</v>
       </c>
       <c r="D37" s="7">
-        <v>4435</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C38" s="4">
-        <v>227</v>
+        <v>2439</v>
       </c>
       <c r="D38" s="7">
-        <v>2104</v>
+        <v>4637</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C39" s="4">
-        <v>2121</v>
+        <v>548</v>
       </c>
       <c r="D39" s="7">
-        <v>4337</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C40" s="4">
-        <v>228</v>
+        <v>2450</v>
       </c>
       <c r="D40" s="7">
-        <v>2099</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C41" s="4">
-        <v>2116</v>
+        <v>324</v>
       </c>
       <c r="D41" s="7">
-        <v>4329</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C42" s="4">
-        <v>1</v>
+        <v>2030</v>
       </c>
       <c r="D42" s="7">
-        <v>1869</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C43" s="4">
-        <v>1886</v>
+        <v>1</v>
       </c>
       <c r="D43" s="7">
-        <v>4102</v>
+        <v>4773</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C44" s="4">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="D44" s="7">
-        <v>1869</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="4">
-        <v>1886</v>
+        <v>2664</v>
       </c>
       <c r="D45" s="7">
-        <v>4087</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C46" s="4">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D46" s="7">
-        <v>1968</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C47" s="4">
-        <v>1985</v>
+        <v>2247</v>
       </c>
       <c r="D47" s="7">
-        <v>4213</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C48" s="4">
-        <v>324</v>
+        <v>1</v>
       </c>
       <c r="D48" s="7">
-        <v>2012</v>
+        <v>5149</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" s="4">
-        <v>2030</v>
+        <v>114</v>
       </c>
       <c r="D49" s="7">
-        <v>4210</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C50" s="4">
-        <v>347</v>
+        <v>2399</v>
       </c>
       <c r="D50" s="7">
-        <v>2179</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C51" s="4">
-        <v>2195</v>
+        <v>1</v>
       </c>
       <c r="D51" s="7">
-        <v>4375</v>
+        <v>5075</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="4">
-        <v>537</v>
+        <v>292</v>
       </c>
       <c r="D52" s="7">
-        <v>2420</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C53" s="4">
-        <v>2439</v>
-      </c>
-      <c r="D53" s="7">
-        <v>4637</v>
+        <v>2388</v>
+      </c>
+      <c r="D53" s="8">
+        <v>4547</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C54" s="4">
-        <v>548</v>
-      </c>
-      <c r="D54" s="7">
-        <v>2431</v>
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4281</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" s="4">
-        <v>2450</v>
+        <v>1</v>
       </c>
       <c r="D55" s="7">
-        <v>4648</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C56" s="4">
-        <v>1</v>
+        <v>1883</v>
       </c>
       <c r="D56" s="7">
-        <v>5596</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C57" s="4">
-        <v>616</v>
+        <v>2668</v>
       </c>
       <c r="D57" s="7">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="4">
-        <v>2624</v>
-      </c>
-      <c r="D58" s="7">
-        <v>4969</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C59" s="4">
-        <v>1</v>
-      </c>
-      <c r="D59" s="7">
-        <v>4773</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="4">
-        <v>122</v>
-      </c>
-      <c r="D60" s="7">
-        <v>2140</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="4">
-        <v>2664</v>
-      </c>
-      <c r="D61" s="7">
-        <v>4427</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="4">
-        <v>1</v>
-      </c>
-      <c r="D62" s="7">
-        <v>4442</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" s="4">
-        <v>2110</v>
-      </c>
-      <c r="D63" s="7">
-        <v>2727</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C64" s="4">
-        <v>811</v>
-      </c>
-      <c r="D64" s="7">
-        <v>2790</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="4">
-        <v>2006</v>
-      </c>
-      <c r="D65" s="7">
-        <v>2725</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C66" s="4">
-        <v>2783</v>
-      </c>
-      <c r="D66" s="7">
-        <v>4273</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67" s="4">
-        <v>1</v>
-      </c>
-      <c r="D67" s="7">
-        <v>6085</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="4">
-        <v>62</v>
-      </c>
-      <c r="D68" s="7">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="4">
-        <v>1330</v>
-      </c>
-      <c r="D69" s="7">
-        <v>3066</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="4">
-        <v>3493</v>
-      </c>
-      <c r="D70" s="7">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="4">
-        <v>1</v>
-      </c>
-      <c r="D71" s="11">
-        <v>4718</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72" s="4">
-        <v>335</v>
-      </c>
-      <c r="D72" s="4">
-        <v>2206</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C73" s="4">
-        <v>2223</v>
-      </c>
-      <c r="D73" s="4">
-        <v>4433</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="4">
-        <v>1</v>
-      </c>
-      <c r="D74" s="4">
         <v>4281</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" s="4">
-        <v>1</v>
-      </c>
-      <c r="D75" s="7">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="4">
-        <v>1883</v>
-      </c>
-      <c r="D76" s="7">
-        <v>2272</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C77" s="4">
-        <v>2668</v>
-      </c>
-      <c r="D77" s="7">
-        <v>4281</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" s="4">
-        <v>1</v>
-      </c>
-      <c r="D78" s="11">
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="4">
-        <v>2594</v>
-      </c>
-      <c r="D79" s="7">
-        <v>3127</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C80" s="4">
-        <v>386</v>
-      </c>
-      <c r="D80" s="7">
-        <v>2083</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C81" s="4">
-        <v>2101</v>
-      </c>
-      <c r="D81" s="7">
-        <v>4278</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C82" s="4">
-        <v>1</v>
-      </c>
-      <c r="D82" s="7">
-        <v>5065</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="4">
-        <v>174</v>
-      </c>
-      <c r="D83" s="7">
-        <v>2252</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C84" s="4">
-        <v>2279</v>
-      </c>
-      <c r="D84" s="7">
-        <v>5038</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="1"/>
     </row>
@@ -5937,6 +5560,9 @@
       <c r="A1520" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1520">
+    <sortCondition ref="A2:A1520"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5948,11 +5574,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4035936-3065-7A4B-90CB-A32C5DA75E1A}">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409643DA-9895-8A4B-8B4F-13B6F889DB87}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD13"/>
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4">
+        <v>321</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2203</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4410</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4035936-3065-7A4B-90CB-A32C5DA75E1A}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6139,6 +5822,342 @@
         <v>5384</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4">
+        <v>206</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2406</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>5257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="4">
+        <v>411</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2998</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>5517</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="4">
+        <v>740</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2661</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3286</v>
+      </c>
+      <c r="D23" s="7">
+        <v>5307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="4">
+        <v>272</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2285</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="4">
+        <v>174</v>
+      </c>
+      <c r="D29" s="7">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2279</v>
+      </c>
+      <c r="D30" s="7">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="4">
+        <v>62</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1330</v>
+      </c>
+      <c r="D33" s="7">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4">
+        <v>3493</v>
+      </c>
+      <c r="D34" s="7">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="7">
+        <v>5596</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="4">
+        <v>616</v>
+      </c>
+      <c r="D36" s="7">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2624</v>
+      </c>
+      <c r="D37" s="7">
+        <v>4969</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>